<commit_message>
Lets discover 'types' in Groovy
</commit_message>
<xml_diff>
--- a/me/2.Something-Groovy.xlsx
+++ b/me/2.Something-Groovy.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gradle\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67251504-50F9-469A-B514-59CE2782711E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F54534-72E3-4A0E-B1DA-E37266F9387C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Starting a Gradle Build Script" sheetId="1" r:id="rId1"/>
     <sheet name="return" sheetId="2" r:id="rId2"/>
+    <sheet name="types" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t>構成</t>
   </si>
@@ -149,6 +150,125 @@
   </si>
   <si>
     <t>②Also return if last line of a method is an assignment</t>
+  </si>
+  <si>
+    <t>int: types</t>
+  </si>
+  <si>
+    <t>Groovy is optional type, which means that we can actually use type or not use them. We have type of varialbe, parameters, return value can be a type or un type. If we declare variable that is</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">un type we need to use the key word is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>def</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can mind that def keyword is synonymous with objectin java. So if declare the variable of type objectin java, it is exactly the same as declaring a variable with the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> word def on groovy</t>
+    </r>
+  </si>
+  <si>
+    <t>we can assign any instance to that particular variable</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> doubleIt(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y = i</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -277,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -290,13 +410,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1323,6 +1441,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>437825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5AC834C-1704-FDC4-7995-29A93556276B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885825" y="1238250"/>
+          <a:ext cx="2600000" cy="1190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>257736</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>98283</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC8F6C6-EB56-C798-2047-BE109301F132}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="671793" y="9391651"/>
+          <a:ext cx="11083178" cy="5565632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3252,18 +3463,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B31BAFB-E4D2-4B19-8710-B54C956F98DC}">
   <dimension ref="A3:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3275,49 +3486,55 @@
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="E7" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="C8" s="12" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="12" t="s">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="E10" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -3327,12 +3544,12 @@
       <c r="H11" s="8"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
@@ -3344,170 +3561,80 @@
       <c r="H15" s="3"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
       <c r="I30" s="6"/>
       <c r="J30" t="s">
         <v>9</v>
@@ -3517,39 +3644,24 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
       <c r="I31" s="6"/>
+      <c r="K31" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
       <c r="I33" s="6"/>
       <c r="J33" t="s">
         <v>9</v>
@@ -3559,29 +3671,17 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="14"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="B35" s="12"/>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="8"/>
@@ -3617,8 +3717,8 @@
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="18" t="s">
+      <c r="A40" s="2"/>
+      <c r="B40" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="3"/>
@@ -3647,68 +3747,26 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="13" t="s">
+      <c r="C42" t="s">
         <v>36</v>
       </c>
       <c r="D42" s="6"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
       <c r="S42" s="6"/>
       <c r="T42" s="6"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="13" t="s">
+      <c r="C43" t="s">
         <v>37</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="13"/>
       <c r="S43" s="6"/>
       <c r="T43" s="6"/>
     </row>
@@ -3717,44 +3775,14 @@
       <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="13"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="13"/>
       <c r="S44" s="6"/>
       <c r="T44" s="6"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="13"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="13"/>
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
     </row>
@@ -3765,394 +3793,91 @@
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="13"/>
       <c r="S46" s="6"/>
       <c r="T46" s="6"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="13"/>
-      <c r="R47" s="13"/>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="13"/>
-      <c r="Q48" s="13"/>
-      <c r="R48" s="13"/>
       <c r="S48" s="6"/>
       <c r="T48" s="6"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="13"/>
-      <c r="P49" s="13"/>
-      <c r="Q49" s="13"/>
-      <c r="R49" s="13"/>
       <c r="S49" s="6"/>
       <c r="T49" s="6"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="13"/>
       <c r="S50" s="6"/>
       <c r="T50" s="6"/>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="13"/>
-      <c r="P51" s="13"/>
-      <c r="Q51" s="13"/>
-      <c r="R51" s="13"/>
       <c r="S51" s="6"/>
       <c r="T51" s="6"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="13"/>
-      <c r="O52" s="13"/>
-      <c r="P52" s="13"/>
-      <c r="Q52" s="13"/>
-      <c r="R52" s="13"/>
       <c r="S52" s="6"/>
       <c r="T52" s="6"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="13"/>
       <c r="S53" s="6"/>
       <c r="T53" s="6"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
-      <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="13"/>
-      <c r="O54" s="13"/>
-      <c r="P54" s="13"/>
-      <c r="Q54" s="13"/>
-      <c r="R54" s="13"/>
       <c r="S54" s="6"/>
       <c r="T54" s="6"/>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="13"/>
-      <c r="O55" s="13"/>
-      <c r="P55" s="13"/>
-      <c r="Q55" s="13"/>
-      <c r="R55" s="13"/>
       <c r="S55" s="6"/>
       <c r="T55" s="6"/>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="13"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="13"/>
-      <c r="R56" s="13"/>
       <c r="S56" s="6"/>
       <c r="T56" s="6"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
-      <c r="L57" s="13"/>
-      <c r="M57" s="13"/>
-      <c r="N57" s="13"/>
-      <c r="O57" s="13"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="13"/>
-      <c r="R57" s="13"/>
       <c r="S57" s="6"/>
       <c r="T57" s="6"/>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="13"/>
-      <c r="L58" s="13"/>
-      <c r="M58" s="13"/>
-      <c r="N58" s="13"/>
-      <c r="O58" s="13"/>
-      <c r="P58" s="13"/>
-      <c r="Q58" s="13"/>
-      <c r="R58" s="13"/>
       <c r="S58" s="6"/>
       <c r="T58" s="6"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="13"/>
-      <c r="N59" s="13"/>
-      <c r="O59" s="13"/>
-      <c r="P59" s="13"/>
-      <c r="Q59" s="13"/>
-      <c r="R59" s="13"/>
       <c r="S59" s="6"/>
       <c r="T59" s="6"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
-      <c r="K60" s="13"/>
-      <c r="L60" s="13"/>
-      <c r="M60" s="13"/>
-      <c r="N60" s="13"/>
-      <c r="O60" s="13"/>
-      <c r="P60" s="13"/>
-      <c r="Q60" s="13"/>
-      <c r="R60" s="13"/>
       <c r="S60" s="6"/>
       <c r="T60" s="6"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
-      <c r="N61" s="13"/>
-      <c r="O61" s="13"/>
-      <c r="P61" s="13"/>
-      <c r="Q61" s="13"/>
-      <c r="R61" s="13"/>
       <c r="S61" s="6"/>
       <c r="T61" s="6"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="13"/>
-      <c r="P62" s="13"/>
-      <c r="Q62" s="13"/>
-      <c r="R62" s="13"/>
       <c r="S62" s="6"/>
       <c r="T62" s="6"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13"/>
-      <c r="O63" s="13"/>
-      <c r="P63" s="13"/>
-      <c r="Q63" s="13"/>
-      <c r="R63" s="13"/>
       <c r="S63" s="6"/>
       <c r="T63" s="6"/>
     </row>
@@ -4180,29 +3905,11 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13"/>
-      <c r="O65" s="13"/>
-      <c r="P65" s="13"/>
-      <c r="Q65" s="13"/>
-      <c r="R65" s="13"/>
-      <c r="S65" s="13"/>
       <c r="T65" s="6"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="B66" s="18" t="s">
+      <c r="B66" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C66" s="3"/>
@@ -4231,92 +3938,36 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="13"/>
-      <c r="R67" s="13"/>
       <c r="S67" s="6"/>
       <c r="T67" s="6"/>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="13" t="s">
+      <c r="C68" t="s">
         <v>36</v>
       </c>
       <c r="D68" s="6"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
-      <c r="P68" s="13"/>
-      <c r="Q68" s="13"/>
-      <c r="R68" s="13"/>
       <c r="S68" s="6"/>
       <c r="T68" s="6"/>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="13" t="s">
+      <c r="C69" t="s">
         <v>37</v>
       </c>
       <c r="D69" s="6"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13"/>
-      <c r="O69" s="13"/>
-      <c r="P69" s="13"/>
-      <c r="Q69" s="13"/>
-      <c r="R69" s="13"/>
       <c r="S69" s="6"/>
       <c r="T69" s="6"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="13" t="s">
+      <c r="C70" t="s">
         <v>38</v>
       </c>
       <c r="D70" s="6"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-      <c r="O70" s="13"/>
-      <c r="P70" s="13"/>
-      <c r="Q70" s="13"/>
-      <c r="R70" s="13"/>
       <c r="S70" s="6"/>
       <c r="T70" s="6"/>
     </row>
@@ -4325,44 +3976,14 @@
       <c r="B71" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C71" s="13"/>
       <c r="D71" s="6"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-      <c r="N71" s="13"/>
-      <c r="O71" s="13"/>
-      <c r="P71" s="13"/>
-      <c r="Q71" s="13"/>
-      <c r="R71" s="13"/>
       <c r="S71" s="6"/>
       <c r="T71" s="6"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
-      <c r="C72" s="13"/>
       <c r="D72" s="6"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="13"/>
-      <c r="N72" s="13"/>
-      <c r="O72" s="13"/>
-      <c r="P72" s="13"/>
-      <c r="Q72" s="13"/>
-      <c r="R72" s="13"/>
       <c r="S72" s="6"/>
       <c r="T72" s="6"/>
     </row>
@@ -4373,372 +3994,86 @@
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="9"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="13"/>
-      <c r="O73" s="13"/>
-      <c r="P73" s="13"/>
-      <c r="Q73" s="13"/>
-      <c r="R73" s="13"/>
       <c r="S73" s="6"/>
       <c r="T73" s="6"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-      <c r="Q74" s="13"/>
-      <c r="R74" s="13"/>
       <c r="S74" s="6"/>
       <c r="T74" s="6"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-      <c r="O75" s="13"/>
-      <c r="P75" s="13"/>
-      <c r="Q75" s="13"/>
-      <c r="R75" s="13"/>
       <c r="S75" s="6"/>
       <c r="T75" s="6"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13"/>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="13"/>
-      <c r="R76" s="13"/>
       <c r="S76" s="6"/>
       <c r="T76" s="6"/>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13"/>
-      <c r="P77" s="13"/>
-      <c r="Q77" s="13"/>
-      <c r="R77" s="13"/>
       <c r="S77" s="6"/>
       <c r="T77" s="6"/>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="13"/>
-      <c r="P78" s="13"/>
-      <c r="Q78" s="13"/>
-      <c r="R78" s="13"/>
       <c r="S78" s="6"/>
       <c r="T78" s="6"/>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="13"/>
-      <c r="N79" s="13"/>
-      <c r="O79" s="13"/>
-      <c r="P79" s="13"/>
-      <c r="Q79" s="13"/>
-      <c r="R79" s="13"/>
       <c r="S79" s="6"/>
       <c r="T79" s="6"/>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="13"/>
-      <c r="R80" s="13"/>
       <c r="S80" s="6"/>
       <c r="T80" s="6"/>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
-      <c r="O81" s="13"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="13"/>
-      <c r="R81" s="13"/>
       <c r="S81" s="6"/>
       <c r="T81" s="6"/>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
-      <c r="O82" s="13"/>
-      <c r="P82" s="13"/>
-      <c r="Q82" s="13"/>
-      <c r="R82" s="13"/>
       <c r="S82" s="6"/>
       <c r="T82" s="6"/>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
-      <c r="O83" s="13"/>
-      <c r="P83" s="13"/>
-      <c r="Q83" s="13"/>
-      <c r="R83" s="13"/>
       <c r="S83" s="6"/>
       <c r="T83" s="6"/>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
-      <c r="N84" s="13"/>
-      <c r="O84" s="13"/>
-      <c r="P84" s="13"/>
-      <c r="Q84" s="13"/>
-      <c r="R84" s="13"/>
       <c r="S84" s="6"/>
       <c r="T84" s="6"/>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
-      <c r="K85" s="13"/>
-      <c r="L85" s="13"/>
-      <c r="M85" s="13"/>
-      <c r="N85" s="13"/>
-      <c r="O85" s="13"/>
-      <c r="P85" s="13"/>
-      <c r="Q85" s="13"/>
-      <c r="R85" s="13"/>
       <c r="S85" s="6"/>
       <c r="T85" s="6"/>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-      <c r="M86" s="13"/>
-      <c r="N86" s="13"/>
-      <c r="O86" s="13"/>
-      <c r="P86" s="13"/>
-      <c r="Q86" s="13"/>
-      <c r="R86" s="13"/>
       <c r="S86" s="6"/>
       <c r="T86" s="6"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="13"/>
-      <c r="M87" s="13"/>
-      <c r="N87" s="13"/>
-      <c r="O87" s="13"/>
-      <c r="P87" s="13"/>
-      <c r="Q87" s="13"/>
-      <c r="R87" s="13"/>
       <c r="S87" s="6"/>
       <c r="T87" s="6"/>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
-      <c r="L88" s="13"/>
-      <c r="M88" s="13"/>
-      <c r="N88" s="13"/>
-      <c r="O88" s="13"/>
-      <c r="P88" s="13"/>
-      <c r="Q88" s="13"/>
-      <c r="R88" s="13"/>
       <c r="S88" s="6"/>
       <c r="T88" s="6"/>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="13"/>
-      <c r="M89" s="13"/>
-      <c r="N89" s="13"/>
-      <c r="O89" s="13"/>
-      <c r="P89" s="13"/>
-      <c r="Q89" s="13"/>
-      <c r="R89" s="13"/>
       <c r="S89" s="6"/>
       <c r="T89" s="6"/>
     </row>
@@ -4790,4 +4125,255 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D4DCD2-143B-4319-8ECA-7D6869C0DF82}">
+  <dimension ref="A3:K48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="E22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I42" s="6"/>
+      <c r="J42" t="s">
+        <v>9</v>
+      </c>
+      <c r="K42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="15"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>